<commit_message>
Add clustering students files
</commit_message>
<xml_diff>
--- a/example/Topic/60/LG/6040i10-2/1/k15/c10d5/W1cW2cW1dW2d-K15C10-clustering.xlsx
+++ b/example/Topic/60/LG/6040i10-2/1/k15/c10d5/W1cW2cW1dW2d-K15C10-clustering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EDU\files\2013\example\Topic\60\LG\6040i10-2\1\k15\c10d5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580B1063-E2A9-48A5-B314-A8AB1DE5ECD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613429E6-3B12-40CF-8D6F-DEED984A1F65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{AD0C68DE-8B8C-4D77-B46E-277C530FD180}"/>
   </bookViews>
@@ -28007,7 +28007,7 @@
   <dimension ref="A1:V87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>